<commit_message>
Update sample spreadsheet with Notes tab
</commit_message>
<xml_diff>
--- a/data/training_attendance.xlsx
+++ b/data/training_attendance.xlsx
@@ -11,6 +11,7 @@
     <sheet name="2016" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2017" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Dates" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Notes" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="73">
   <si>
     <t xml:space="preserve">RDM training</t>
   </si>
@@ -223,18 +224,35 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added data for 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2016 tab, added Delivered By column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summarized 2016 data in Dates tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added data for 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\ MMM"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="167" formatCode="D\ MMM\ "/>
-    <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -242,6 +260,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -263,16 +282,19 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -280,6 +302,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -372,7 +395,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,10 +504,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,10 +516,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -522,10 +537,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,23 +559,23 @@
   </sheetPr>
   <dimension ref="B2:L38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.07142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,25 +1480,25 @@
   </sheetPr>
   <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.5765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.5765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.0255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2142857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="27" min="13" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="19.4387755102041"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="13" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="0" width="19.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1623,7 +1634,7 @@
       </c>
       <c r="J4" s="24" t="n">
         <f aca="false">RANDBETWEEN(15,I4)</f>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K4" s="24" t="s">
         <v>14</v>
@@ -1667,7 +1678,7 @@
       </c>
       <c r="J5" s="22" t="n">
         <f aca="false">RANDBETWEEN(15,I5)</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K5" s="22" t="s">
         <v>14</v>
@@ -1734,13 +1745,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16"/>
-      <c r="B7" s="27" t="n">
+      <c r="B7" s="25" t="n">
         <v>42797</v>
       </c>
       <c r="C7" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="27" t="n">
+      <c r="D7" s="25" t="n">
         <v>36600</v>
       </c>
       <c r="E7" s="22" t="s">
@@ -1758,7 +1769,7 @@
       </c>
       <c r="J7" s="22" t="n">
         <f aca="false">RANDBETWEEN(15,I7)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>14</v>
@@ -1782,7 +1793,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="16"/>
-      <c r="B8" s="27" t="n">
+      <c r="B8" s="25" t="n">
         <v>42798</v>
       </c>
       <c r="C8" s="22" t="n">
@@ -1806,7 +1817,7 @@
       </c>
       <c r="J8" s="22" t="n">
         <f aca="false">RANDBETWEEN(15,I8)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K8" s="22" t="s">
         <v>48</v>
@@ -1830,7 +1841,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="16"/>
-      <c r="B9" s="27" t="n">
+      <c r="B9" s="25" t="n">
         <v>42833</v>
       </c>
       <c r="C9" s="22" t="n">
@@ -1843,17 +1854,17 @@
         <v>49</v>
       </c>
       <c r="F9" s="16"/>
-      <c r="G9" s="28" t="n">
+      <c r="G9" s="27" t="n">
         <v>42827</v>
       </c>
-      <c r="H9" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="29" t="n">
+      <c r="H9" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="28" t="n">
         <v>41</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29" t="s">
+      <c r="J9" s="28"/>
+      <c r="K9" s="28" t="s">
         <v>48</v>
       </c>
       <c r="L9" s="16"/>
@@ -1875,7 +1886,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="16"/>
-      <c r="B10" s="27" t="n">
+      <c r="B10" s="25" t="n">
         <v>42881</v>
       </c>
       <c r="C10" s="22" t="n">
@@ -1899,7 +1910,7 @@
       </c>
       <c r="J10" s="22" t="n">
         <f aca="false">RANDBETWEEN(15,I10)</f>
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="K10" s="22" t="s">
         <v>14</v>
@@ -1929,7 +1940,7 @@
       <c r="C11" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="27" t="n">
+      <c r="D11" s="25" t="n">
         <v>36580</v>
       </c>
       <c r="E11" s="22" t="s">
@@ -1947,7 +1958,7 @@
       </c>
       <c r="J11" s="22" t="n">
         <f aca="false">RANDBETWEEN(15,I11)</f>
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K11" s="22" t="s">
         <v>48</v>
@@ -1971,33 +1982,33 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="16"/>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="30" t="n">
+      <c r="C12" s="29" t="n">
         <v>1.5</v>
       </c>
-      <c r="D12" s="31" t="n">
+      <c r="D12" s="30" t="n">
         <v>38180</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="29" t="s">
         <v>49</v>
       </c>
       <c r="F12" s="16"/>
-      <c r="G12" s="32" t="n">
+      <c r="G12" s="30" t="n">
         <v>42902</v>
       </c>
-      <c r="H12" s="30" t="n">
+      <c r="H12" s="29" t="n">
         <v>1</v>
       </c>
       <c r="I12" s="15" t="n">
         <v>15</v>
       </c>
-      <c r="J12" s="30" t="n">
+      <c r="J12" s="29" t="n">
         <f aca="false">RANDBETWEEN(15,I12)</f>
         <v>15</v>
       </c>
-      <c r="K12" s="30" t="s">
+      <c r="K12" s="29" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="16"/>
@@ -2128,40 +2139,40 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33" t="s">
+    <row r="1" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="33" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2172,16 +2183,16 @@
       <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="37" t="n">
+      <c r="C2" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="35" t="n">
         <v>26</v>
       </c>
-      <c r="E2" s="36" t="n">
+      <c r="E2" s="34" t="n">
         <v>17</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -2195,16 +2206,16 @@
       <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="37" t="n">
+      <c r="C3" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="35" t="n">
         <v>38</v>
       </c>
-      <c r="E3" s="36" t="n">
+      <c r="E3" s="34" t="n">
         <v>20</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -2218,16 +2229,16 @@
       <c r="B4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="37" t="n">
+      <c r="C4" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="35" t="n">
         <v>19</v>
       </c>
-      <c r="E4" s="36" t="n">
+      <c r="E4" s="34" t="n">
         <v>25</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="34" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="0" t="s">
@@ -2241,16 +2252,16 @@
       <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="37" t="n">
+      <c r="C5" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="35" t="n">
         <v>27</v>
       </c>
-      <c r="E5" s="36" t="n">
+      <c r="E5" s="34" t="n">
         <v>24</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -2264,16 +2275,16 @@
       <c r="B6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="37" t="n">
+      <c r="C6" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="35" t="n">
         <v>32</v>
       </c>
-      <c r="E6" s="36" t="n">
+      <c r="E6" s="34" t="n">
         <v>20</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="34" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -2287,16 +2298,16 @@
       <c r="B7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="38" t="n">
+      <c r="C7" s="34" t="n">
         <v>1.5</v>
       </c>
-      <c r="D7" s="38" t="n">
+      <c r="D7" s="34" t="n">
         <v>41</v>
       </c>
-      <c r="E7" s="38" t="n">
+      <c r="E7" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="34" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -2310,16 +2321,16 @@
       <c r="B8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="36" t="n">
+      <c r="C8" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="37" t="n">
+      <c r="D8" s="35" t="n">
         <v>44</v>
       </c>
-      <c r="E8" s="36" t="n">
+      <c r="E8" s="34" t="n">
         <v>22</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="0" t="s">
@@ -2333,16 +2344,16 @@
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="37" t="n">
+      <c r="C9" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="35" t="n">
         <v>43</v>
       </c>
-      <c r="E9" s="36" t="n">
+      <c r="E9" s="34" t="n">
         <v>31</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="34" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="0" t="s">
@@ -2356,16 +2367,16 @@
       <c r="B10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="36" t="n">
+      <c r="C10" s="34" t="n">
         <v>1.5</v>
       </c>
-      <c r="D10" s="37" t="n">
+      <c r="D10" s="35" t="n">
         <v>1.5</v>
       </c>
-      <c r="E10" s="36" t="n">
+      <c r="E10" s="34" t="n">
         <v>15</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="0" t="s">
@@ -2657,4 +2668,73 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:C7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove RANDBETWEEN from sample spreadsheet
</commit_message>
<xml_diff>
--- a/data/training_attendance.xlsx
+++ b/data/training_attendance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" state="visible" r:id="rId2"/>
@@ -559,8 +559,8 @@
   </sheetPr>
   <dimension ref="B2:L38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1480,8 +1480,8 @@
   </sheetPr>
   <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1633,7 +1633,6 @@
         <v>26</v>
       </c>
       <c r="J4" s="24" t="n">
-        <f aca="false">RANDBETWEEN(15,I4)</f>
         <v>23</v>
       </c>
       <c r="K4" s="24" t="s">
@@ -1677,7 +1676,6 @@
         <v>38</v>
       </c>
       <c r="J5" s="22" t="n">
-        <f aca="false">RANDBETWEEN(15,I5)</f>
         <v>26</v>
       </c>
       <c r="K5" s="22" t="s">
@@ -1768,7 +1766,6 @@
         <v>27</v>
       </c>
       <c r="J7" s="22" t="n">
-        <f aca="false">RANDBETWEEN(15,I7)</f>
         <v>17</v>
       </c>
       <c r="K7" s="22" t="s">
@@ -1816,7 +1813,6 @@
         <v>32</v>
       </c>
       <c r="J8" s="22" t="n">
-        <f aca="false">RANDBETWEEN(15,I8)</f>
         <v>15</v>
       </c>
       <c r="K8" s="22" t="s">
@@ -1909,7 +1905,6 @@
         <v>44</v>
       </c>
       <c r="J10" s="22" t="n">
-        <f aca="false">RANDBETWEEN(15,I10)</f>
         <v>44</v>
       </c>
       <c r="K10" s="22" t="s">
@@ -1957,7 +1952,6 @@
         <v>43</v>
       </c>
       <c r="J11" s="22" t="n">
-        <f aca="false">RANDBETWEEN(15,I11)</f>
         <v>37</v>
       </c>
       <c r="K11" s="22" t="s">
@@ -2005,7 +1999,6 @@
         <v>15</v>
       </c>
       <c r="J12" s="29" t="n">
-        <f aca="false">RANDBETWEEN(15,I12)</f>
         <v>15</v>
       </c>
       <c r="K12" s="29" t="s">

</xml_diff>

<commit_message>
Change delimiters in sample data file
</commit_message>
<xml_diff>
--- a/data/training_attendance.xlsx
+++ b/data/training_attendance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Length (hours)</t>
   </si>
   <si>
-    <t xml:space="preserve">PGR/PDRA/other</t>
+    <t xml:space="preserve">PGR|PDRA|other</t>
   </si>
   <si>
     <t xml:space="preserve">Delivered by</t>
@@ -559,8 +559,8 @@
   </sheetPr>
   <dimension ref="B2:L38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1480,8 +1480,8 @@
   </sheetPr>
   <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>